<commit_message>
update config tiktok project
</commit_message>
<xml_diff>
--- a/reactjs.xlsx
+++ b/reactjs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="2"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MENU" sheetId="3" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="285">
   <si>
     <t>react là 1 thư viện javascript</t>
   </si>
@@ -631,9 +631,6 @@
   </si>
   <si>
     <t xml:space="preserve">thêm react route vào </t>
-  </si>
-  <si>
-    <t>bug</t>
   </si>
   <si>
     <t>sau khi xong nên dọn dẹp để khỏi rò rỉ bộ nhớ</t>
@@ -889,12 +886,51 @@
   <si>
     <t xml:space="preserve">useReducer sử dụng cho các component phức tạp </t>
   </si>
+  <si>
+    <t>1. cài đặt thư viện để webpack : "cutomize-cra"</t>
+  </si>
+  <si>
+    <t>2. cài đặt babel plugin</t>
+  </si>
+  <si>
+    <t>cài sass</t>
+  </si>
+  <si>
+    <t>reset css normalize npm</t>
+  </si>
+  <si>
+    <t>npm install --save normalize.css</t>
+  </si>
+  <si>
+    <t xml:space="preserve">extension tạo tắt function componet </t>
+  </si>
+  <si>
+    <t>extenstion gom nhóm "htmltagwrap"</t>
+  </si>
+  <si>
+    <t>callback</t>
+  </si>
+  <si>
+    <t>là hàm (function) được truyền qua đối số khi gọi hàm khác</t>
+  </si>
+  <si>
+    <t>thư viện className</t>
+  </si>
+  <si>
+    <t>npm i classnames</t>
+  </si>
+  <si>
+    <t>npm i -D sass</t>
+  </si>
+  <si>
+    <t>npm i customize-cra react-app-rewired -D</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -982,6 +1018,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF1F2328"/>
+      <name val="Var(--fontStack-monospace, ui-m"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1004,7 +1051,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1031,6 +1078,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1186,13 +1240,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>256</xdr:row>
+      <xdr:row>269</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>275</xdr:row>
+      <xdr:row>288</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1224,13 +1278,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>276</xdr:row>
+      <xdr:row>289</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>295</xdr:row>
+      <xdr:row>308</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1262,13 +1316,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>298</xdr:row>
+      <xdr:row>311</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>328</xdr:row>
+      <xdr:row>341</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1288,6 +1342,44 @@
         <a:xfrm>
           <a:off x="1219200" y="54854475"/>
           <a:ext cx="7000875" cy="5734050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>114299</xdr:colOff>
+      <xdr:row>257</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>267</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1333499" y="49110900"/>
+          <a:ext cx="2705101" cy="1914525"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1739,9 +1831,9 @@
       <selection activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:14">
       <c r="B2">
         <v>1</v>
       </c>
@@ -1749,42 +1841,42 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:14">
       <c r="D3" s="7" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:14">
       <c r="N4" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:14">
       <c r="N5" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:14">
       <c r="N6" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:14">
       <c r="N7" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:14">
       <c r="N8" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:14">
       <c r="N9" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:14">
       <c r="B11">
         <v>1</v>
       </c>
@@ -1792,12 +1884,12 @@
         <v>182</v>
       </c>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:14">
       <c r="D12" s="1" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:14">
       <c r="D13" s="1" t="s">
         <v>184</v>
       </c>
@@ -1805,75 +1897,75 @@
         <v>186</v>
       </c>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:14">
       <c r="D14" s="1" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:14">
       <c r="C16" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:4">
       <c r="D17" s="1" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:4">
       <c r="D18" s="1" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:4">
       <c r="C20" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:4">
       <c r="D21" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:4">
       <c r="C23" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="47" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:3">
       <c r="C47" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="48" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:3">
       <c r="C48" s="12" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="49" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:6">
       <c r="D49" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="50" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="4:6">
       <c r="D50" t="s">
         <v>26</v>
       </c>
       <c r="F50" s="11"/>
     </row>
-    <row r="51" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="4:6">
       <c r="D51" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="52" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="4:6">
       <c r="D52" s="8" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="53" spans="4:6" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="53" spans="4:6">
       <c r="D53" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -1887,34 +1979,98 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B3:T9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="3" spans="2:20">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>272</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="4" spans="2:20">
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="5" spans="2:20">
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>274</v>
+      </c>
+      <c r="H5" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="6" spans="2:20" ht="15.75">
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>275</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="7" spans="2:20">
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>281</v>
+      </c>
+      <c r="H7" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="8" spans="2:20">
+      <c r="T8" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="9" spans="2:20">
+      <c r="T9" t="s">
+        <v>278</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:W334"/>
+  <dimension ref="B2:W347"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A202" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P216" sqref="P216"/>
+    <sheetView topLeftCell="A241" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I264" sqref="I264"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10">
       <c r="D2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10">
       <c r="I4" s="4" t="s">
         <v>3</v>
       </c>
@@ -1922,7 +2078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10">
       <c r="I5" s="4" t="s">
         <v>3</v>
       </c>
@@ -1930,7 +2086,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10">
       <c r="I6" s="4" t="s">
         <v>3</v>
       </c>
@@ -1938,7 +2094,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10">
       <c r="I7" s="4" t="s">
         <v>3</v>
       </c>
@@ -1946,7 +2102,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10">
       <c r="I8" s="4" t="s">
         <v>3</v>
       </c>
@@ -1954,7 +2110,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10">
       <c r="I9" s="4" t="s">
         <v>3</v>
       </c>
@@ -1962,7 +2118,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10">
       <c r="I10" s="4" t="s">
         <v>3</v>
       </c>
@@ -1970,17 +2126,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10">
       <c r="I12" s="10" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10">
       <c r="B13" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10">
       <c r="C14" s="2" t="s">
         <v>3</v>
       </c>
@@ -1988,7 +2144,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10">
       <c r="C15" s="2" t="s">
         <v>3</v>
       </c>
@@ -1996,7 +2152,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10">
       <c r="C16" s="2" t="s">
         <v>3</v>
       </c>
@@ -2004,7 +2160,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:13">
       <c r="C17" s="2" t="s">
         <v>3</v>
       </c>
@@ -2012,12 +2168,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:13">
       <c r="D19" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:13">
       <c r="B20" s="1" t="s">
         <v>12</v>
       </c>
@@ -2025,7 +2181,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:13">
       <c r="B22" s="1" t="s">
         <v>14</v>
       </c>
@@ -2036,7 +2192,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:13">
       <c r="C24" s="2" t="s">
         <v>3</v>
       </c>
@@ -2047,7 +2203,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:13">
       <c r="C25" s="2" t="s">
         <v>3</v>
       </c>
@@ -2058,13 +2214,13 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:13">
       <c r="C26" s="2"/>
       <c r="E26" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:13">
       <c r="C27" s="2" t="s">
         <v>3</v>
       </c>
@@ -2072,16 +2228,16 @@
         <v>17</v>
       </c>
       <c r="F27" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13">
       <c r="C28" s="2"/>
       <c r="E28" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:13">
       <c r="C29" s="2"/>
       <c r="E29" s="4" t="s">
         <v>53</v>
@@ -2090,7 +2246,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:13">
       <c r="C30" s="2"/>
       <c r="E30" s="4" t="s">
         <v>53</v>
@@ -2099,7 +2255,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:13">
       <c r="C31" s="2"/>
       <c r="E31" s="4" t="s">
         <v>53</v>
@@ -2108,40 +2264,40 @@
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:13">
       <c r="C32" s="2"/>
       <c r="E32" s="4" t="s">
         <v>53</v>
       </c>
       <c r="F32" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="33" spans="3:6">
       <c r="C33" s="2"/>
       <c r="E33" s="4" t="s">
         <v>53</v>
       </c>
       <c r="F33" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="34" spans="3:6">
       <c r="C34" s="2"/>
       <c r="E34" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:6">
       <c r="C35" s="2"/>
       <c r="E35" s="4" t="s">
         <v>53</v>
       </c>
       <c r="F35" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="36" spans="3:6" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="36" spans="3:6">
       <c r="C36" s="2"/>
       <c r="E36" s="4" t="s">
         <v>53</v>
@@ -2150,7 +2306,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:6">
       <c r="C37" s="2"/>
       <c r="E37" s="4" t="s">
         <v>53</v>
@@ -2159,40 +2315,40 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:6">
       <c r="C38" s="2"/>
       <c r="E38" s="4" t="s">
         <v>53</v>
       </c>
       <c r="F38" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="39" spans="3:6" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="39" spans="3:6">
       <c r="C39" s="2"/>
       <c r="E39" s="4" t="s">
         <v>53</v>
       </c>
       <c r="F39" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="40" spans="3:6" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="40" spans="3:6">
       <c r="C40" s="2"/>
       <c r="E40" s="4" t="s">
         <v>53</v>
       </c>
       <c r="F40" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="41" spans="3:6" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="41" spans="3:6">
       <c r="C41" s="2"/>
       <c r="E41" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:6">
       <c r="C42" s="2"/>
       <c r="E42" s="4" t="s">
         <v>53</v>
@@ -2201,34 +2357,34 @@
         <v>36</v>
       </c>
     </row>
-    <row r="43" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:6">
       <c r="C43" s="2"/>
       <c r="E43" s="4" t="s">
         <v>53</v>
       </c>
       <c r="F43" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="44" spans="3:6" x14ac:dyDescent="0.25">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="44" spans="3:6">
       <c r="C44" s="2"/>
       <c r="E44" s="4" t="s">
         <v>53</v>
       </c>
       <c r="F44" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="45" spans="3:6" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="45" spans="3:6">
       <c r="C45" s="2"/>
       <c r="E45" s="4" t="s">
         <v>53</v>
       </c>
       <c r="F45" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="46" spans="3:6" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="46" spans="3:6">
       <c r="C46" s="2" t="s">
         <v>3</v>
       </c>
@@ -2236,7 +2392,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="47" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:6">
       <c r="C47" s="2"/>
       <c r="E47" t="s">
         <v>38</v>
@@ -2245,37 +2401,37 @@
         <v>88</v>
       </c>
     </row>
-    <row r="48" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:6">
       <c r="C48" s="2"/>
       <c r="E48" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="49" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:6">
       <c r="C49" s="2"/>
       <c r="E49" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="50" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:6">
       <c r="C50" s="2"/>
       <c r="E50" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="51" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:6">
       <c r="C51" s="2"/>
       <c r="E51" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="52" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:6">
       <c r="C52" s="2"/>
       <c r="E52" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="53" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:6">
       <c r="C53" s="2" t="s">
         <v>3</v>
       </c>
@@ -2283,19 +2439,19 @@
         <v>18</v>
       </c>
     </row>
-    <row r="54" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:6">
       <c r="C54" s="2"/>
       <c r="E54" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="55" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:6">
       <c r="C55" s="2"/>
       <c r="E55" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="56" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:6">
       <c r="C56" s="2" t="s">
         <v>3</v>
       </c>
@@ -2303,22 +2459,22 @@
         <v>45</v>
       </c>
     </row>
-    <row r="57" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:6">
       <c r="C57" s="2"/>
       <c r="E57" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="58" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:6">
       <c r="C58" s="2"/>
       <c r="E58" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="59" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:6">
       <c r="C59" s="2"/>
     </row>
-    <row r="60" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:6">
       <c r="C60" s="2" t="s">
         <v>3</v>
       </c>
@@ -2329,13 +2485,13 @@
         <v>77</v>
       </c>
     </row>
-    <row r="61" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:6">
       <c r="C61" s="2"/>
       <c r="E61" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="62" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:6">
       <c r="C62" s="2"/>
       <c r="E62" s="4" t="s">
         <v>53</v>
@@ -2344,7 +2500,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="63" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:6">
       <c r="C63" s="2"/>
       <c r="E63" s="4" t="s">
         <v>53</v>
@@ -2353,13 +2509,13 @@
         <v>79</v>
       </c>
     </row>
-    <row r="64" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:6">
       <c r="C64" s="2"/>
       <c r="E64" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:6">
       <c r="C65" s="2"/>
       <c r="E65" s="2" t="s">
         <v>53</v>
@@ -2368,7 +2524,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:6">
       <c r="C66" s="2"/>
       <c r="E66" s="2" t="s">
         <v>53</v>
@@ -2377,7 +2533,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:6">
       <c r="C67" s="2" t="s">
         <v>3</v>
       </c>
@@ -2388,7 +2544,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:6">
       <c r="C68" s="2" t="s">
         <v>3</v>
       </c>
@@ -2396,7 +2552,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:6">
       <c r="B69" s="1" t="s">
         <v>56</v>
       </c>
@@ -2404,19 +2560,19 @@
         <v>54</v>
       </c>
     </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:6">
       <c r="B70" s="1"/>
       <c r="C70" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:6">
       <c r="B71" s="1"/>
       <c r="C71" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:6">
       <c r="C72" s="2" t="s">
         <v>3</v>
       </c>
@@ -2424,7 +2580,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:6">
       <c r="C73" s="2" t="s">
         <v>3</v>
       </c>
@@ -2432,7 +2588,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:6">
       <c r="C74" s="2" t="s">
         <v>3</v>
       </c>
@@ -2440,7 +2596,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:6">
       <c r="C75" s="2" t="s">
         <v>3</v>
       </c>
@@ -2448,37 +2604,37 @@
         <v>59</v>
       </c>
     </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:6">
       <c r="B77" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:6">
       <c r="D78" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:6">
       <c r="D79" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="80" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:6">
       <c r="D80" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="81" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:19">
       <c r="D81" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="82" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:19">
       <c r="B82" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="84" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:19">
       <c r="B84" s="1" t="s">
         <v>61</v>
       </c>
@@ -2489,15 +2645,15 @@
         <v>195</v>
       </c>
     </row>
-    <row r="85" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:19">
       <c r="C85" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D85" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="86" spans="2:19" x14ac:dyDescent="0.25">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="86" spans="2:19">
       <c r="C86" s="4" t="s">
         <v>3</v>
       </c>
@@ -2508,12 +2664,12 @@
         <v>196</v>
       </c>
     </row>
-    <row r="87" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:19">
       <c r="C87" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D87" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="R87" t="s">
         <v>197</v>
@@ -2522,7 +2678,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="88" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:19">
       <c r="B88" s="1" t="s">
         <v>63</v>
       </c>
@@ -2530,23 +2686,23 @@
         <v>64</v>
       </c>
     </row>
-    <row r="89" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:19">
       <c r="C89" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D89" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="90" spans="2:19">
+      <c r="C90" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D90" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="90" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="C90" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D90" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="91" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:19">
       <c r="B91" s="1" t="s">
         <v>65</v>
       </c>
@@ -2554,12 +2710,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="93" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:19">
       <c r="B93" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="94" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:19">
       <c r="C94" s="4" t="s">
         <v>3</v>
       </c>
@@ -2567,7 +2723,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="95" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:19">
       <c r="C95" s="4" t="s">
         <v>3</v>
       </c>
@@ -2575,12 +2731,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="97" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:23">
       <c r="B97" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="98" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:23">
       <c r="C98" s="2" t="s">
         <v>3</v>
       </c>
@@ -2588,15 +2744,15 @@
         <v>90</v>
       </c>
     </row>
-    <row r="99" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:23">
       <c r="C99" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D99" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="100" spans="2:23" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="100" spans="2:23">
       <c r="B100" s="1" t="s">
         <v>68</v>
       </c>
@@ -2607,7 +2763,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="101" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:23">
       <c r="C101" s="2" t="s">
         <v>3</v>
       </c>
@@ -2621,7 +2777,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="102" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:23">
       <c r="C102" s="2"/>
       <c r="D102" s="4" t="s">
         <v>53</v>
@@ -2633,7 +2789,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="103" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:23">
       <c r="C103" s="2"/>
       <c r="D103" s="4" t="s">
         <v>53</v>
@@ -2642,58 +2798,58 @@
         <v>106</v>
       </c>
     </row>
-    <row r="104" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:23">
       <c r="C104" s="2"/>
     </row>
-    <row r="105" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:23">
       <c r="C105" s="2"/>
     </row>
-    <row r="106" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:23">
       <c r="C106" s="2"/>
     </row>
-    <row r="107" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:23">
       <c r="C107" s="2"/>
     </row>
-    <row r="108" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:23">
       <c r="C108" s="2"/>
     </row>
-    <row r="109" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:23">
       <c r="C109" s="2"/>
     </row>
-    <row r="110" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:23">
       <c r="C110" s="2"/>
     </row>
-    <row r="111" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:23">
       <c r="C111" s="2"/>
     </row>
-    <row r="112" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:23">
       <c r="C112" s="2"/>
     </row>
-    <row r="113" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:4" ht="15.75" customHeight="1">
       <c r="C113" s="2"/>
     </row>
-    <row r="114" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:4" ht="15.75" customHeight="1">
       <c r="C114" s="2"/>
     </row>
-    <row r="115" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:4" ht="15.75" customHeight="1">
       <c r="C115" s="2"/>
     </row>
-    <row r="116" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:4" ht="15.75" customHeight="1">
       <c r="C116" s="2"/>
     </row>
-    <row r="117" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:4" ht="15.75" customHeight="1">
       <c r="C117" s="2"/>
     </row>
-    <row r="118" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:4" ht="15.75" customHeight="1">
       <c r="C118" s="2"/>
     </row>
-    <row r="119" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:4" ht="15.75" customHeight="1">
       <c r="C119" s="2"/>
     </row>
-    <row r="120" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:4">
       <c r="C120" s="2"/>
     </row>
-    <row r="121" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:4">
       <c r="B121" s="1" t="s">
         <v>69</v>
       </c>
@@ -2701,136 +2857,136 @@
         <v>92</v>
       </c>
     </row>
-    <row r="123" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:4">
       <c r="B123" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="125" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:4">
       <c r="B125" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="126" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:4">
       <c r="B126" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="127" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:4">
       <c r="B127" s="1"/>
       <c r="D127" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="128" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:4">
       <c r="B128" s="1"/>
       <c r="D128" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="129" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:4">
       <c r="B129" s="1"/>
       <c r="D129" s="9" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="130" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:4">
       <c r="B130" s="1"/>
       <c r="D130" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="131" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:4">
       <c r="B131" s="1"/>
       <c r="D131" s="9" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="132" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:4">
       <c r="B132" s="1"/>
       <c r="D132" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="133" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:4">
       <c r="B133" s="1"/>
       <c r="D133" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="134" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:4">
       <c r="B134" s="1"/>
       <c r="D134" s="9" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="135" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:4">
       <c r="B135" s="1"/>
       <c r="D135" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="136" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:4">
       <c r="B136" s="1"/>
       <c r="D136" s="9" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="137" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:4">
       <c r="B137" s="1"/>
       <c r="D137" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="138" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:4">
       <c r="B138" s="1"/>
       <c r="D138" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="139" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:4">
       <c r="B139" s="1"/>
       <c r="D139" s="9" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="140" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:4">
       <c r="D140" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="141" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:4">
       <c r="D141" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="142" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:4">
       <c r="B142" s="1"/>
       <c r="D142" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="143" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:4">
       <c r="D143" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="145" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:11">
       <c r="B145" s="8" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="146" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:11">
       <c r="D146" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="147" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:11">
       <c r="D147" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="149" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:11">
       <c r="B149" s="8" t="s">
         <v>72</v>
       </c>
@@ -2838,7 +2994,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="150" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:11">
       <c r="B150" s="8"/>
       <c r="C150" s="4" t="s">
         <v>3</v>
@@ -2847,7 +3003,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="151" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:11">
       <c r="B151" s="8"/>
       <c r="C151" s="4" t="s">
         <v>3</v>
@@ -2856,28 +3012,28 @@
         <v>144</v>
       </c>
     </row>
-    <row r="152" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:11">
       <c r="B152" s="8"/>
       <c r="D152" s="5"/>
       <c r="E152" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="153" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:11">
       <c r="B153" s="8"/>
       <c r="D153" s="5"/>
       <c r="E153" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="154" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:11">
       <c r="B154" s="8"/>
       <c r="D154" s="5"/>
       <c r="E154" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="155" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:11">
       <c r="B155" t="s">
         <v>50</v>
       </c>
@@ -2885,7 +3041,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="156" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:11">
       <c r="C156" s="13" t="s">
         <v>3</v>
       </c>
@@ -2893,7 +3049,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="157" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:11">
       <c r="C157" s="13" t="s">
         <v>3</v>
       </c>
@@ -2901,7 +3057,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="158" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:11">
       <c r="C158" s="13" t="s">
         <v>3</v>
       </c>
@@ -2909,7 +3065,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="159" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:11">
       <c r="B159" t="s">
         <v>50</v>
       </c>
@@ -2917,18 +3073,18 @@
         <v>96</v>
       </c>
     </row>
-    <row r="160" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:11">
       <c r="C160" s="13" t="s">
         <v>3</v>
       </c>
       <c r="D160" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="K160" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="161" spans="3:7" x14ac:dyDescent="0.25">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="161" spans="3:7">
       <c r="C161" s="13" t="s">
         <v>3</v>
       </c>
@@ -2936,15 +3092,15 @@
         <v>151</v>
       </c>
     </row>
-    <row r="162" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="162" spans="3:7">
       <c r="C162" s="13" t="s">
         <v>3</v>
       </c>
       <c r="D162" s="14" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="163" spans="3:7" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="163" spans="3:7">
       <c r="C163" s="13" t="s">
         <v>3</v>
       </c>
@@ -2952,7 +3108,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="164" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="164" spans="3:7">
       <c r="C164" s="13" t="s">
         <v>3</v>
       </c>
@@ -2960,28 +3116,28 @@
         <v>153</v>
       </c>
     </row>
-    <row r="165" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="165" spans="3:7">
       <c r="C165" s="13" t="s">
         <v>3</v>
       </c>
       <c r="D165" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="166" spans="3:7" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="166" spans="3:7">
       <c r="C166" s="13" t="s">
         <v>3</v>
       </c>
       <c r="D166" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="167" spans="3:7" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="167" spans="3:7">
       <c r="C167" s="13" t="s">
         <v>3</v>
       </c>
       <c r="D167" s="10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E167" s="15"/>
       <c r="F167" s="15" t="s">
@@ -2989,12 +3145,12 @@
       </c>
       <c r="G167" s="15"/>
     </row>
-    <row r="168" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="168" spans="3:7">
       <c r="C168" s="13" t="s">
         <v>3</v>
       </c>
       <c r="D168" s="10" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E168" s="15" t="s">
         <v>50</v>
@@ -3002,146 +3158,146 @@
       <c r="F168" s="15"/>
       <c r="G168" s="15"/>
     </row>
-    <row r="169" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="169" spans="3:7">
       <c r="C169" s="13" t="s">
         <v>3</v>
       </c>
       <c r="D169" s="10" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E169" s="15"/>
       <c r="F169" s="15"/>
       <c r="G169" s="15"/>
     </row>
-    <row r="170" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="170" spans="3:7">
       <c r="C170" s="13"/>
       <c r="D170" s="4" t="s">
         <v>53</v>
       </c>
       <c r="E170" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F170" s="15"/>
       <c r="G170" s="15"/>
     </row>
-    <row r="171" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="171" spans="3:7">
       <c r="C171" s="13"/>
       <c r="D171" s="4" t="s">
         <v>53</v>
       </c>
       <c r="E171" s="15" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F171" s="15"/>
       <c r="G171" s="15"/>
     </row>
-    <row r="172" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="172" spans="3:7">
       <c r="C172" s="13" t="s">
         <v>3</v>
       </c>
       <c r="D172" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E172" s="15"/>
       <c r="F172" s="15"/>
       <c r="G172" s="15"/>
     </row>
-    <row r="173" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="173" spans="3:7">
       <c r="C173" s="13"/>
       <c r="D173" s="4" t="s">
         <v>53</v>
       </c>
       <c r="E173" s="15" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F173" s="15"/>
       <c r="G173" s="15"/>
     </row>
-    <row r="174" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="174" spans="3:7">
       <c r="C174" s="13"/>
       <c r="D174" s="4" t="s">
         <v>53</v>
       </c>
       <c r="E174" s="15" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F174" s="15"/>
       <c r="G174" s="15"/>
     </row>
-    <row r="175" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="175" spans="3:7">
       <c r="C175" s="13" t="s">
         <v>3</v>
       </c>
       <c r="D175" s="10" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="176" spans="3:7">
+      <c r="C176" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D176" s="10" t="s">
         <v>252</v>
-      </c>
-    </row>
-    <row r="176" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C176" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D176" s="10" t="s">
-        <v>253</v>
       </c>
       <c r="F176" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="177" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:7">
       <c r="C177" s="13" t="s">
         <v>3</v>
       </c>
       <c r="D177" s="10" t="s">
+        <v>253</v>
+      </c>
+      <c r="F177" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="178" spans="2:7">
+      <c r="C178" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D178" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="F177" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="178" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C178" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D178" s="10" t="s">
-        <v>255</v>
-      </c>
       <c r="G178" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="179" spans="2:7" x14ac:dyDescent="0.25">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="179" spans="2:7">
       <c r="C179" s="13" t="s">
         <v>3</v>
       </c>
       <c r="D179" s="10" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="180" spans="2:7">
+      <c r="C180" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D180" s="10" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="180" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C180" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D180" s="10" t="s">
+    <row r="181" spans="2:7">
+      <c r="C181" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D181" s="10" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="181" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C181" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D181" s="10" t="s">
+    <row r="182" spans="2:7">
+      <c r="C182" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D182" s="10" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="182" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C182" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D182" s="10" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="183" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:7">
       <c r="B183" t="s">
         <v>50</v>
       </c>
@@ -3149,23 +3305,23 @@
         <v>97</v>
       </c>
     </row>
-    <row r="184" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="184" spans="2:7">
       <c r="C184" s="13" t="s">
         <v>3</v>
       </c>
       <c r="D184" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="185" spans="2:7" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="185" spans="2:7">
       <c r="C185" s="13" t="s">
         <v>3</v>
       </c>
       <c r="D185" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="186" spans="2:7" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="186" spans="2:7">
       <c r="C186" s="13" t="s">
         <v>3</v>
       </c>
@@ -3173,7 +3329,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="187" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:7">
       <c r="C187" s="13" t="s">
         <v>3</v>
       </c>
@@ -3181,43 +3337,43 @@
         <v>155</v>
       </c>
     </row>
-    <row r="188" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:7">
       <c r="C188" s="13"/>
       <c r="D188" s="4" t="s">
         <v>53</v>
       </c>
       <c r="E188" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="189" spans="2:7" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="189" spans="2:7">
       <c r="C189" s="13"/>
       <c r="D189" s="4" t="s">
         <v>53</v>
       </c>
       <c r="E189" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="190" spans="2:7" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="190" spans="2:7">
       <c r="C190" s="13"/>
       <c r="D190" s="4" t="s">
         <v>53</v>
       </c>
       <c r="E190" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="191" spans="2:7" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="191" spans="2:7">
       <c r="C191" s="13"/>
       <c r="D191" s="4" t="s">
         <v>53</v>
       </c>
       <c r="E191" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="192" spans="2:7" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="192" spans="2:7">
       <c r="B192" t="s">
         <v>50</v>
       </c>
@@ -3225,18 +3381,18 @@
         <v>98</v>
       </c>
       <c r="D192" s="10" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="193" spans="3:5">
+      <c r="C193" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D193" s="10" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="193" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C193" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D193" s="10" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="194" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="3:5">
       <c r="C194" s="13" t="s">
         <v>3</v>
       </c>
@@ -3244,7 +3400,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="195" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="3:5">
       <c r="C195" s="13" t="s">
         <v>3</v>
       </c>
@@ -3252,7 +3408,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="196" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="3:5">
       <c r="C196" s="13" t="s">
         <v>3</v>
       </c>
@@ -3260,7 +3416,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="197" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="3:5">
       <c r="C197" s="13"/>
       <c r="D197" s="4" t="s">
         <v>53</v>
@@ -3269,7 +3425,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="198" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="3:5">
       <c r="C198" s="13"/>
       <c r="D198" s="4" t="s">
         <v>53</v>
@@ -3278,7 +3434,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="199" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="3:5">
       <c r="C199" s="13"/>
       <c r="D199" s="4" t="s">
         <v>53</v>
@@ -3287,23 +3443,23 @@
         <v>161</v>
       </c>
     </row>
-    <row r="200" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="200" spans="3:5">
       <c r="C200" s="13" t="s">
         <v>3</v>
       </c>
       <c r="D200" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="201" spans="3:5" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="201" spans="3:5">
       <c r="C201" s="13"/>
     </row>
-    <row r="202" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="3:5">
       <c r="C202" s="6" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="203" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="203" spans="3:5">
       <c r="C203" s="13" t="s">
         <v>3</v>
       </c>
@@ -3311,7 +3467,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="204" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="3:5">
       <c r="C204" s="13" t="s">
         <v>3</v>
       </c>
@@ -3319,7 +3475,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="205" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="205" spans="3:5">
       <c r="C205" s="13" t="s">
         <v>3</v>
       </c>
@@ -3327,28 +3483,28 @@
         <v>164</v>
       </c>
     </row>
-    <row r="206" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="206" spans="3:5">
       <c r="C206" s="13" t="s">
         <v>3</v>
       </c>
       <c r="D206" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="207" spans="3:5">
+      <c r="C207" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D207" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="207" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C207" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D207" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="208" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="208" spans="3:5">
       <c r="C208" s="6" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="209" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="209" spans="3:8">
       <c r="C209" s="13" t="s">
         <v>3</v>
       </c>
@@ -3359,7 +3515,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="210" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="210" spans="3:8">
       <c r="C210" s="13" t="s">
         <v>3</v>
       </c>
@@ -3367,7 +3523,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="211" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="211" spans="3:8">
       <c r="C211" s="13" t="s">
         <v>3</v>
       </c>
@@ -3375,7 +3531,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="212" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="212" spans="3:8">
       <c r="C212" s="13" t="s">
         <v>3</v>
       </c>
@@ -3383,7 +3539,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="213" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="213" spans="3:8">
       <c r="C213" s="13" t="s">
         <v>3</v>
       </c>
@@ -3391,7 +3547,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="214" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="214" spans="3:8">
       <c r="C214" s="13" t="s">
         <v>3</v>
       </c>
@@ -3399,7 +3555,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="215" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="215" spans="3:8">
       <c r="C215" s="13" t="s">
         <v>3</v>
       </c>
@@ -3407,12 +3563,12 @@
         <v>172</v>
       </c>
     </row>
-    <row r="216" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="216" spans="3:8">
       <c r="C216" s="6" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="217" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="217" spans="3:8">
       <c r="C217" s="13" t="s">
         <v>3</v>
       </c>
@@ -3420,7 +3576,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="218" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="218" spans="3:8">
       <c r="C218" s="13" t="s">
         <v>3</v>
       </c>
@@ -3428,7 +3584,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="219" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="219" spans="3:8">
       <c r="C219" s="13" t="s">
         <v>3</v>
       </c>
@@ -3436,7 +3592,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="220" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="220" spans="3:8">
       <c r="C220" s="13" t="s">
         <v>3</v>
       </c>
@@ -3444,20 +3600,20 @@
         <v>175</v>
       </c>
     </row>
-    <row r="221" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="221" spans="3:8">
       <c r="C221" s="13" t="s">
         <v>3</v>
       </c>
       <c r="D221" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="222" spans="3:8" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="222" spans="3:8">
       <c r="C222" s="6" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="223" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="223" spans="3:8">
       <c r="C223" s="13" t="s">
         <v>3</v>
       </c>
@@ -3465,7 +3621,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="224" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="224" spans="3:8">
       <c r="C224" s="13" t="s">
         <v>3</v>
       </c>
@@ -3473,78 +3629,88 @@
         <v>177</v>
       </c>
     </row>
-    <row r="226" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C226" s="13" t="s">
+    <row r="226" spans="2:5">
+      <c r="C226" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="D226" t="s">
         <v>236</v>
       </c>
-      <c r="D226" t="s">
+    </row>
+    <row r="227" spans="2:5">
+      <c r="D227" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="229" spans="2:5">
+      <c r="C229" s="16" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="227" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D227" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="229" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C229" s="13" t="s">
+      <c r="E229" t="s">
         <v>238</v>
       </c>
-      <c r="E229" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="232" spans="2:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="232" spans="2:5">
       <c r="B232" s="8" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="256" spans="2:2">
+      <c r="B256" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="257" spans="2:3">
+      <c r="C257" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="269" spans="2:3">
+      <c r="B269" s="8" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="256" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B256" s="8" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="298" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B298" s="8" t="s">
+    <row r="311" spans="2:4">
+      <c r="B311" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="D311" t="s">
         <v>250</v>
       </c>
-      <c r="D298" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="331" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B331" t="s">
-        <v>3</v>
-      </c>
-      <c r="C331" t="s">
+    </row>
+    <row r="344" spans="2:9">
+      <c r="B344" t="s">
+        <v>3</v>
+      </c>
+      <c r="C344" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="345" spans="2:9">
+      <c r="D345" t="s">
+        <v>72</v>
+      </c>
+      <c r="I345" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="346" spans="2:9">
+      <c r="C346" t="s">
+        <v>268</v>
+      </c>
+      <c r="D346" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="332" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D332" t="s">
-        <v>72</v>
-      </c>
-      <c r="I332" t="s">
+      <c r="E346" t="s">
+        <v>264</v>
+      </c>
+      <c r="I346" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="333" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C333" t="s">
-        <v>269</v>
-      </c>
-      <c r="D333" t="s">
-        <v>264</v>
-      </c>
-      <c r="E333" t="s">
+    <row r="347" spans="2:9">
+      <c r="D347" t="s">
         <v>265</v>
-      </c>
-      <c r="I333" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="334" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D334" t="s">
-        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -3556,20 +3722,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:I29"/>
+  <dimension ref="C2:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:9">
       <c r="C2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:9">
       <c r="D3" s="1" t="s">
         <v>127</v>
       </c>
@@ -3577,7 +3743,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="4" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:9">
       <c r="D4" s="1" t="s">
         <v>129</v>
       </c>
@@ -3585,7 +3751,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:9">
       <c r="D5" s="1" t="s">
         <v>130</v>
       </c>
@@ -3593,7 +3759,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:9">
       <c r="D6" s="1" t="s">
         <v>140</v>
       </c>
@@ -3601,7 +3767,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:9">
       <c r="D7" s="1" t="s">
         <v>199</v>
       </c>
@@ -3609,33 +3775,28 @@
         <v>200</v>
       </c>
     </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:9">
       <c r="D8" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="I8" t="s">
         <v>230</v>
       </c>
-      <c r="I8" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="3:9">
       <c r="D9" s="1" t="s">
         <v>129</v>
       </c>
       <c r="I9" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="10" spans="3:9">
+      <c r="D10" s="1" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D10" s="1" t="s">
-        <v>233</v>
-      </c>
       <c r="I10" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="29" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C29" t="s">
-        <v>201</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -3652,9 +3813,9 @@
       <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="5" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:3">
       <c r="C5" t="s">
         <v>104</v>
       </c>

</xml_diff>